<commit_message>
adjusted card layout for large description and two cards added.
</commit_message>
<xml_diff>
--- a/strats-sources/commonStrats.xlsx
+++ b/strats-sources/commonStrats.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\micro\gitrepos\w40k-strat-card\strats-sources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC9C39AE-CE5E-4131-B304-96B8E3DC99A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7CCBA37-53A2-4A12-949E-796371DEBE59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{3DE3896D-95B2-400C-96E2-85A96F1479CA}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="23">
   <si>
     <t>Timing</t>
   </si>
@@ -61,12 +61,6 @@
     <t>Relance de commandement</t>
   </si>
   <si>
-    <t>Jet, de touche, svg, avance, charge, psy, abjurer, nombre attaque</t>
-  </si>
-  <si>
-    <t>Utilisez ce stratagème après que vous ayez effectué un jet de touche, blessure, dégats, sauvegarde, Avance, charge, psy, abjurer ou nombre d'attaque effectuées par une arme. &lt;strong&gt;Relancez ce jet ou ce test&lt;/strong&gt;.</t>
-  </si>
-  <si>
     <t>PageReference</t>
   </si>
   <si>
@@ -83,6 +77,33 @@
   </si>
   <si>
     <t>strats-sources\assets\base-rulebook.png</t>
+  </si>
+  <si>
+    <t>Utilisez ce stratag&amp;egrave;me apr&amp;egrave;s que vous ayez effectu&amp;eacute; un jet de touche, blessure, d&amp;eacute;gats, sauvegarde, Avance, charge, psy, abjurer ou nombre d'attaque effectu&amp;eacute;es par une arme. &lt;strong&gt;Relancez ce jet ou ce test&lt;/strong&gt;.</t>
+  </si>
+  <si>
+    <t>Apr&amp;egrave; jet touche, svg, avance, charge, psy, abjurer, nombre attaque</t>
+  </si>
+  <si>
+    <t>Exterminez-les</t>
+  </si>
+  <si>
+    <t>Unit&amp;eacute; ennemie bat en retraite</t>
+  </si>
+  <si>
+    <t>Utilisez ce stratag&amp;egrave;me quand une unit&amp;eacute; ennemie bat en retraite, avant que la moindre figurine de l'unt&amp;eacute; soit d&amp;eacute;plac&amp;eacute;e.&lt;br/&gt;Jetez 1D6 pour chaque figurine se trouvant &amp;agrave; d'engagement de l'unit&amp;eacute; ennemie ; pour chaque r&amp;eacute;sultat de 6, l'unit&amp;eacute; ennemie subit 1 blessure mortelle.</t>
+  </si>
+  <si>
+    <t>Repli desesp&amp;eacute;r&amp;eacute;</t>
+  </si>
+  <si>
+    <t>Phase de mouvement</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>Choisir une unit&amp;eacute; qui ne s'est pas d&amp;eacute;plac&amp;eacute; &amp;agrave; port&amp;eacute;e d'engagement d'aun moins une unit&amp;eacute; ennemie.&lt;br/&gt;&lt;strong&gt;Jetez 1D6&lt;/strong&gt; pour chaque fig de l'unit&amp;eacute; finie. &lt;strong&gt;Sur 1 l'unit&amp;eacute est d&amp;eacute;truite&lt;/strong&gt;. Si l'unit&amp;eacute; n'est pas d&amp;eacute;truite elle peut tenter de &lt;i&gt;Battre en Retraite&lt;/i&gt;.&lt;br/&gt;Si la figurine termine son mouvement &amp;agrave; &lt;i&gt;Port&amp;eacute;e d'Engagement&lt;/i&gt;, elle d&amp;eacute;truite.&lt;br/&gt;&lt;strong&gt;L'unit&amp;eacute; ne peut plus rien faire&lt;/strong&gt;, m&amp;ecirc;me si elle a une r&amp;egrave;gle qui lui permet de faire actions apr&amp;egrave; avoir Battu en Retraite.</t>
   </si>
 </sst>
 </file>
@@ -437,10 +458,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0B88374-B535-46D0-A48E-0EFF11686FCD}">
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+    <sheetView tabSelected="1" topLeftCell="B3" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="59.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -464,7 +485,7 @@
         <v>1</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>6</v>
@@ -476,30 +497,82 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="C2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="H2" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="90" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="F3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="G3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="G2" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>15</v>
+    </row>
+    <row r="4" spans="1:8" ht="165" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>